<commit_message>
add whatapp recharge screen, profile update
</commit_message>
<xml_diff>
--- a/backend/public/StudentSampleData.xlsx
+++ b/backend/public/StudentSampleData.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\the_v\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63FEB990-EC7B-415B-B3C0-246780EB208C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,48 +16,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>mobile</t>
-  </si>
-  <si>
-    <t>whatsapp</t>
-  </si>
-  <si>
-    <t>dob</t>
-  </si>
-  <si>
-    <t>state</t>
-  </si>
-  <si>
-    <t>city</t>
-  </si>
-  <si>
-    <t>sex</t>
-  </si>
-  <si>
-    <t>pincode</t>
-  </si>
-  <si>
-    <t>highestQualifcation</t>
-  </si>
-  <si>
-    <t>address</t>
-  </si>
-  <si>
-    <t>Experienced</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Roll No</t>
+  </si>
+  <si>
+    <t>Father Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Course </t>
+  </si>
+  <si>
+    <t>Session</t>
+  </si>
+  <si>
+    <t>College</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -396,41 +372,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.44140625" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.109375" customWidth="1"/>
-    <col min="11" max="11" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="14.21875" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -443,24 +419,6 @@
       </c>
       <c r="F1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -470,7 +428,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -478,14 +436,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -493,7 +451,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>